<commit_message>
Antwortsatz hinzugefügt, Formatierung überarbeitet
</commit_message>
<xml_diff>
--- a/Orga/Nutzwertanalyse.xlsx
+++ b/Orga/Nutzwertanalyse.xlsx
@@ -1,20 +1,21 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
-  <workbookPr defaultThemeVersion="153222"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="21328"/>
+  <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="F:\Projekt\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Moshbit\source\repos\myTodo\Orga\"/>
     </mc:Choice>
   </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D5BB36B4-6201-4585-A0EF-2B0C10035001}" xr6:coauthVersionLast="41" xr6:coauthVersionMax="41" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="12615"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="16440" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Tabelle1" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="152511"/>
+  <calcPr calcId="181029"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -38,9 +39,6 @@
     <t>Gesamt</t>
   </si>
   <si>
-    <t>Fertige to Do App</t>
-  </si>
-  <si>
     <t>Desktop Version</t>
   </si>
   <si>
@@ -62,20 +60,23 @@
     <t>Feature: Reminding</t>
   </si>
   <si>
-    <t>Feature: Verschiebbarkeit von Kategorien</t>
-  </si>
-  <si>
     <t>Feature: Availability</t>
   </si>
   <si>
     <t>Marktvolumen</t>
+  </si>
+  <si>
+    <t>Smartphone App</t>
+  </si>
+  <si>
+    <t>Feature: Verschieben von Kategorien</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="3" x14ac:knownFonts="1">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+  <fonts count="4" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -92,7 +93,15 @@
     </font>
     <font>
       <b/>
-      <sz val="11"/>
+      <sz val="14"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="12"/>
       <color theme="1"/>
       <name val="Calibri"/>
       <family val="2"/>
@@ -119,7 +128,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="9">
+  <borders count="14">
     <border>
       <left/>
       <right/>
@@ -128,10 +137,81 @@
       <diagonal/>
     </border>
     <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
       <left style="medium">
         <color indexed="64"/>
       </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
       <right style="medium">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
         <color indexed="64"/>
       </right>
       <top style="medium">
@@ -143,29 +223,85 @@
       <diagonal/>
     </border>
     <border>
-      <left/>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right/>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right/>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
       <right/>
       <top style="medium">
         <color indexed="64"/>
       </top>
-      <bottom/>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="medium">
-        <color indexed="64"/>
-      </left>
-      <right/>
-      <top style="medium">
-        <color indexed="64"/>
-      </top>
       <bottom style="medium">
         <color indexed="64"/>
       </bottom>
       <diagonal/>
     </border>
     <border>
-      <left/>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
       <right style="medium">
         <color indexed="64"/>
       </right>
@@ -173,58 +309,6 @@
         <color indexed="64"/>
       </top>
       <bottom style="medium">
-        <color indexed="64"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="thin">
-        <color indexed="64"/>
-      </left>
-      <right style="thin">
-        <color indexed="64"/>
-      </right>
-      <top style="thin">
-        <color indexed="64"/>
-      </top>
-      <bottom style="thin">
-        <color indexed="64"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
-      <right style="thin">
-        <color indexed="64"/>
-      </right>
-      <top style="thin">
-        <color indexed="64"/>
-      </top>
-      <bottom style="thin">
-        <color indexed="64"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="medium">
-        <color indexed="64"/>
-      </left>
-      <right style="medium">
-        <color indexed="64"/>
-      </right>
-      <top/>
-      <bottom/>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="thin">
-        <color indexed="64"/>
-      </left>
-      <right style="thin">
-        <color indexed="64"/>
-      </right>
-      <top/>
-      <bottom style="thin">
         <color indexed="64"/>
       </bottom>
       <diagonal/>
@@ -234,40 +318,58 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="15">
+  <cellXfs count="21">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="9" fontId="0" fillId="0" borderId="3" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="9" fontId="0" fillId="0" borderId="5" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1"/>
+    <xf numFmtId="9" fontId="0" fillId="0" borderId="8" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="9" fontId="0" fillId="0" borderId="6" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="1" fontId="0" fillId="0" borderId="6" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="9" fontId="0" fillId="0" borderId="5" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="9" fontId="0" fillId="2" borderId="6" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="9" fontId="0" fillId="3" borderId="6" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="9" fontId="0" fillId="0" borderId="11" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="9" fontId="3" fillId="0" borderId="12" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="1" fontId="3" fillId="0" borderId="6" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="9" fontId="3" fillId="3" borderId="13" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="9" fontId="3" fillId="2" borderId="13" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
   </cellXfs>
@@ -286,6 +388,92 @@
     </ext>
   </extLst>
 </styleSheet>
+</file>
+
+<file path=xl/drawings/drawing1.xml><?xml version="1.0" encoding="utf-8"?>
+<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>1</xdr:col>
+      <xdr:colOff>400050</xdr:colOff>
+      <xdr:row>14</xdr:row>
+      <xdr:rowOff>76200</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>5</xdr:col>
+      <xdr:colOff>581025</xdr:colOff>
+      <xdr:row>20</xdr:row>
+      <xdr:rowOff>28575</xdr:rowOff>
+    </xdr:to>
+    <xdr:sp macro="" textlink="">
+      <xdr:nvSpPr>
+        <xdr:cNvPr id="2" name="Textfeld 1">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{2A636402-34AC-4FFF-8E09-25AA547EAE40}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvSpPr txBox="1"/>
+      </xdr:nvSpPr>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="2695575" y="2905125"/>
+          <a:ext cx="3609975" cy="1095375"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:solidFill>
+          <a:schemeClr val="lt1"/>
+        </a:solidFill>
+        <a:ln w="9525" cmpd="sng">
+          <a:solidFill>
+            <a:schemeClr val="lt1">
+              <a:shade val="50000"/>
+            </a:schemeClr>
+          </a:solidFill>
+        </a:ln>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="0">
+          <a:scrgbClr r="0" g="0" b="0"/>
+        </a:lnRef>
+        <a:fillRef idx="0">
+          <a:scrgbClr r="0" g="0" b="0"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:scrgbClr r="0" g="0" b="0"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="dk1"/>
+        </a:fontRef>
+      </xdr:style>
+      <xdr:txBody>
+        <a:bodyPr vertOverflow="clip" horzOverflow="clip" wrap="square" rtlCol="0" anchor="t"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:r>
+            <a:rPr lang="de-DE" sz="2000" b="1"/>
+            <a:t>Ergebnis der NWA:</a:t>
+          </a:r>
+        </a:p>
+        <a:p>
+          <a:r>
+            <a:rPr lang="de-DE" sz="2000"/>
+            <a:t>Eine Smartphone App ist vorerst das geeignetere</a:t>
+          </a:r>
+          <a:r>
+            <a:rPr lang="de-DE" sz="2000" baseline="0"/>
+            <a:t> Medium.</a:t>
+          </a:r>
+          <a:endParaRPr lang="de-DE" sz="2000"/>
+        </a:p>
+      </xdr:txBody>
+    </xdr:sp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+</xdr:wsDr>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -550,273 +738,271 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:F13"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D13" sqref="D13"/>
+      <selection activeCell="I21" sqref="I21"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="37.85546875" customWidth="1"/>
-    <col min="2" max="2" width="14.85546875" customWidth="1"/>
-    <col min="4" max="4" width="16.28515625" customWidth="1"/>
-    <col min="6" max="6" width="16.7109375" customWidth="1"/>
+    <col min="1" max="1" width="34.42578125" bestFit="1" customWidth="1"/>
+    <col min="2" max="6" width="12.85546875" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:6" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
-    <row r="2" spans="1:6" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A2" s="5"/>
-      <c r="B2" s="1"/>
+    <row r="2" spans="1:6" ht="18.75" x14ac:dyDescent="0.3">
+      <c r="A2" s="6"/>
+      <c r="B2" s="6"/>
       <c r="C2" s="8" t="s">
+        <v>13</v>
+      </c>
+      <c r="D2" s="9"/>
+      <c r="E2" s="8" t="s">
         <v>4</v>
       </c>
-      <c r="D2" s="2"/>
-      <c r="E2" s="8" t="s">
+      <c r="F2" s="9"/>
+    </row>
+    <row r="3" spans="1:6" ht="21" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A3" s="12" t="s">
+        <v>0</v>
+      </c>
+      <c r="B3" s="13" t="s">
+        <v>1</v>
+      </c>
+      <c r="C3" s="14" t="s">
+        <v>2</v>
+      </c>
+      <c r="D3" s="15" t="s">
+        <v>3</v>
+      </c>
+      <c r="E3" s="14" t="s">
+        <v>2</v>
+      </c>
+      <c r="F3" s="15" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="4" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A4" s="5" t="s">
         <v>5</v>
       </c>
-      <c r="F2" s="2"/>
-    </row>
-    <row r="3" spans="1:6" ht="21" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A3" s="5" t="s">
-        <v>0</v>
-      </c>
-      <c r="B3" s="4" t="s">
-        <v>1</v>
-      </c>
-      <c r="C3" s="7" t="s">
-        <v>2</v>
-      </c>
-      <c r="D3" s="7" t="s">
-        <v>3</v>
-      </c>
-      <c r="E3" s="7" t="s">
-        <v>2</v>
-      </c>
-      <c r="F3" s="7" t="s">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="4" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A4" s="6" t="s">
-        <v>6</v>
-      </c>
-      <c r="B4" s="10">
+      <c r="B4" s="7">
         <v>0.15</v>
       </c>
-      <c r="C4" s="3">
+      <c r="C4" s="1">
         <v>90</v>
       </c>
-      <c r="D4" s="12">
+      <c r="D4" s="2">
         <f>B4*C4/100</f>
         <v>0.13500000000000001</v>
       </c>
-      <c r="E4" s="3">
+      <c r="E4" s="1">
         <v>100</v>
       </c>
-      <c r="F4" s="12">
+      <c r="F4" s="2">
         <f>B4*E4/100</f>
         <v>0.15</v>
       </c>
     </row>
     <row r="5" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A5" s="6" t="s">
-        <v>13</v>
-      </c>
-      <c r="B5" s="10">
+      <c r="A5" s="5" t="s">
+        <v>11</v>
+      </c>
+      <c r="B5" s="7">
         <v>0.1</v>
       </c>
-      <c r="C5" s="3">
+      <c r="C5" s="1">
         <v>100</v>
       </c>
-      <c r="D5" s="12">
+      <c r="D5" s="2">
         <f t="shared" ref="D5:D12" si="0">B5*C5/100</f>
         <v>0.1</v>
       </c>
-      <c r="E5" s="3">
+      <c r="E5" s="1">
         <v>40</v>
       </c>
-      <c r="F5" s="12">
+      <c r="F5" s="2">
         <f t="shared" ref="F5:F12" si="1">B5*E5/100</f>
         <v>0.04</v>
       </c>
     </row>
     <row r="6" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A6" s="6" t="s">
-        <v>11</v>
-      </c>
-      <c r="B6" s="10">
+      <c r="A6" s="5" t="s">
+        <v>10</v>
+      </c>
+      <c r="B6" s="7">
         <v>0.18</v>
       </c>
-      <c r="C6" s="3">
+      <c r="C6" s="1">
         <v>100</v>
       </c>
-      <c r="D6" s="12">
+      <c r="D6" s="2">
         <f t="shared" si="0"/>
         <v>0.18</v>
       </c>
-      <c r="E6" s="3">
+      <c r="E6" s="1">
         <v>30</v>
       </c>
-      <c r="F6" s="12">
+      <c r="F6" s="2">
         <f t="shared" si="1"/>
         <v>5.3999999999999992E-2</v>
       </c>
     </row>
     <row r="7" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A7" s="6" t="s">
-        <v>10</v>
-      </c>
-      <c r="B7" s="10">
+      <c r="A7" s="5" t="s">
+        <v>9</v>
+      </c>
+      <c r="B7" s="7">
         <v>0.05</v>
       </c>
-      <c r="C7" s="3">
+      <c r="C7" s="1">
         <v>100</v>
       </c>
-      <c r="D7" s="12">
+      <c r="D7" s="2">
         <f t="shared" si="0"/>
         <v>0.05</v>
       </c>
-      <c r="E7" s="3">
+      <c r="E7" s="1">
         <v>100</v>
       </c>
-      <c r="F7" s="12">
+      <c r="F7" s="2">
         <f t="shared" si="1"/>
         <v>0.05</v>
       </c>
     </row>
     <row r="8" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A8" s="6" t="s">
-        <v>12</v>
-      </c>
-      <c r="B8" s="10">
+      <c r="A8" s="5" t="s">
+        <v>14</v>
+      </c>
+      <c r="B8" s="7">
         <v>0.05</v>
       </c>
-      <c r="C8" s="3">
+      <c r="C8" s="1">
         <v>100</v>
       </c>
-      <c r="D8" s="12">
+      <c r="D8" s="2">
         <f t="shared" si="0"/>
         <v>0.05</v>
       </c>
-      <c r="E8" s="3">
+      <c r="E8" s="1">
         <v>100</v>
       </c>
-      <c r="F8" s="12">
+      <c r="F8" s="2">
         <f t="shared" si="1"/>
         <v>0.05</v>
       </c>
     </row>
     <row r="9" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A9" s="6" t="s">
-        <v>7</v>
-      </c>
-      <c r="B9" s="10">
+      <c r="A9" s="5" t="s">
+        <v>6</v>
+      </c>
+      <c r="B9" s="7">
         <v>0.1</v>
       </c>
-      <c r="C9" s="3">
+      <c r="C9" s="1">
         <v>90</v>
       </c>
-      <c r="D9" s="12">
+      <c r="D9" s="2">
         <f t="shared" si="0"/>
         <v>0.09</v>
       </c>
-      <c r="E9" s="3">
+      <c r="E9" s="1">
         <v>100</v>
       </c>
-      <c r="F9" s="12">
+      <c r="F9" s="2">
         <f t="shared" si="1"/>
         <v>0.1</v>
       </c>
     </row>
     <row r="10" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A10" s="6" t="s">
-        <v>14</v>
-      </c>
-      <c r="B10" s="10">
+      <c r="A10" s="5" t="s">
+        <v>12</v>
+      </c>
+      <c r="B10" s="7">
         <v>0.18</v>
       </c>
-      <c r="C10" s="3">
+      <c r="C10" s="1">
         <v>100</v>
       </c>
-      <c r="D10" s="12">
+      <c r="D10" s="2">
         <f t="shared" si="0"/>
         <v>0.18</v>
       </c>
-      <c r="E10" s="3">
+      <c r="E10" s="1">
         <v>30</v>
       </c>
-      <c r="F10" s="12">
+      <c r="F10" s="2">
         <f t="shared" si="1"/>
         <v>5.3999999999999992E-2</v>
       </c>
     </row>
     <row r="11" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A11" s="6" t="s">
-        <v>9</v>
-      </c>
-      <c r="B11" s="10">
+      <c r="A11" s="5" t="s">
+        <v>8</v>
+      </c>
+      <c r="B11" s="7">
         <v>0.05</v>
       </c>
-      <c r="C11" s="3">
+      <c r="C11" s="1">
         <v>70</v>
       </c>
-      <c r="D11" s="12">
+      <c r="D11" s="2">
         <f t="shared" si="0"/>
         <v>3.5000000000000003E-2</v>
       </c>
-      <c r="E11" s="3">
+      <c r="E11" s="1">
         <v>90</v>
       </c>
-      <c r="F11" s="12">
+      <c r="F11" s="2">
         <f t="shared" si="1"/>
         <v>4.4999999999999998E-2</v>
       </c>
     </row>
     <row r="12" spans="1:6" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A12" s="6" t="s">
-        <v>8</v>
-      </c>
-      <c r="B12" s="10">
+      <c r="A12" s="10" t="s">
+        <v>7</v>
+      </c>
+      <c r="B12" s="11">
         <v>0.14000000000000001</v>
       </c>
       <c r="C12" s="3">
         <v>90</v>
       </c>
-      <c r="D12" s="12">
+      <c r="D12" s="4">
         <f t="shared" si="0"/>
         <v>0.126</v>
       </c>
       <c r="E12" s="3">
         <v>100</v>
       </c>
-      <c r="F12" s="12">
+      <c r="F12" s="4">
         <f t="shared" si="1"/>
         <v>0.14000000000000001</v>
       </c>
     </row>
-    <row r="13" spans="1:6" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A13" s="9" t="s">
+    <row r="13" spans="1:6" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A13" s="16" t="s">
         <v>3</v>
       </c>
-      <c r="B13" s="10">
+      <c r="B13" s="17">
         <f>SUM(B4:B12)</f>
         <v>1</v>
       </c>
-      <c r="C13" s="11">
+      <c r="C13" s="18">
         <f t="shared" ref="C13:F13" si="2">SUM(C4:C12)</f>
         <v>840</v>
       </c>
-      <c r="D13" s="14">
+      <c r="D13" s="19">
         <f t="shared" si="2"/>
         <v>0.94599999999999995</v>
       </c>
-      <c r="E13" s="11">
+      <c r="E13" s="18">
         <f t="shared" si="2"/>
         <v>690</v>
       </c>
-      <c r="F13" s="13">
+      <c r="F13" s="20">
         <f t="shared" si="2"/>
         <v>0.68299999999999994</v>
       </c>
@@ -831,5 +1017,6 @@
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.78740157499999996" bottom="0.78740157499999996" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
+  <drawing r:id="rId2"/>
 </worksheet>
 </file>
</xml_diff>